<commit_message>
add new code for segment test
Test code for segment powers each LED independently with a delay
in-between. Code used to test update time and delay using high FPS go
pro footage
</commit_message>
<xml_diff>
--- a/calcs_ports_timers.xlsx
+++ b/calcs_ports_timers.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="460" windowWidth="14100" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14100" yWindow="460" windowWidth="14100" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PINS" sheetId="5" r:id="rId1"/>
-    <sheet name="PHYSICAL" sheetId="7" r:id="rId2"/>
-    <sheet name="TIMERS" sheetId="2" r:id="rId3"/>
-    <sheet name="REGISTERS" sheetId="3" r:id="rId4"/>
-    <sheet name="TIMING" sheetId="4" r:id="rId5"/>
+    <sheet name="SEGMENTS" sheetId="8" r:id="rId2"/>
+    <sheet name="PHYSICAL" sheetId="7" r:id="rId3"/>
+    <sheet name="TIMERS" sheetId="2" r:id="rId4"/>
+    <sheet name="REGISTERS" sheetId="3" r:id="rId5"/>
+    <sheet name="TIMING" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="104">
   <si>
     <t>Wheel size</t>
   </si>
@@ -364,13 +365,25 @@
   </si>
   <si>
     <t>ANALOG</t>
+  </si>
+  <si>
+    <t>SNUM</t>
+  </si>
+  <si>
+    <t>LEDNUM</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>CAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +406,22 @@
       <sz val="7"/>
       <color theme="1"/>
       <name val="HelveticaLTStd"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -448,8 +477,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -464,7 +497,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,15 +825,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -813,7 +850,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -823,8 +860,12 @@
       <c r="D2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <f>A2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -834,8 +875,12 @@
       <c r="D3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f t="shared" ref="F3:F25" si="0">A3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>16</v>
       </c>
@@ -848,8 +893,12 @@
       <c r="E4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>17</v>
       </c>
@@ -862,8 +911,12 @@
       <c r="E5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -873,16 +926,24 @@
       <c r="E6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>19</v>
       </c>
@@ -895,8 +956,12 @@
       <c r="E8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>18</v>
       </c>
@@ -906,8 +971,12 @@
       <c r="E9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>15</v>
       </c>
@@ -920,8 +989,12 @@
       <c r="E10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>22</v>
       </c>
@@ -931,8 +1004,12 @@
       <c r="E11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>23</v>
       </c>
@@ -942,8 +1019,12 @@
       <c r="E12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -953,8 +1034,12 @@
       <c r="E13" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -964,8 +1049,12 @@
       <c r="E14" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -978,8 +1067,12 @@
       <c r="E15" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>11</v>
       </c>
@@ -989,8 +1082,12 @@
       <c r="E16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1000,8 +1097,12 @@
       <c r="E17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1011,8 +1112,12 @@
       <c r="E18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>14</v>
       </c>
@@ -1022,8 +1127,12 @@
       <c r="E19" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1033,8 +1142,12 @@
       <c r="E20" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1044,8 +1157,12 @@
       <c r="E21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6</v>
       </c>
@@ -1055,8 +1172,12 @@
       <c r="E22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1066,8 +1187,12 @@
       <c r="E23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1077,8 +1202,12 @@
       <c r="E24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1087,6 +1216,10 @@
       </c>
       <c r="E25" t="s">
         <v>87</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1099,10 +1232,968 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50:F65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>13</v>
+      </c>
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>15</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50">
+        <f>VLOOKUP(C50,PINS!E$11:F$25,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50">
+        <f>VLOOKUP(E50,PINS!E$11:F$25,2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51">
+        <f>VLOOKUP(C51,PINS!E$11:F$25,2,0)</f>
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51">
+        <f>VLOOKUP(E51,PINS!E$11:F$25,2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52">
+        <f>VLOOKUP(C52,PINS!E$11:F$25,2,0)</f>
+        <v>21</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52">
+        <f>VLOOKUP(E52,PINS!E$11:F$25,2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53">
+        <f>VLOOKUP(C53,PINS!E$11:F$25,2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53">
+        <f>VLOOKUP(E53,PINS!E$11:F$25,2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54">
+        <f>VLOOKUP(C54,PINS!E$11:F$25,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54">
+        <f>VLOOKUP(E54,PINS!E$11:F$25,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55">
+        <f>VLOOKUP(C55,PINS!E$11:F$25,2,0)</f>
+        <v>20</v>
+      </c>
+      <c r="E55" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55">
+        <f>VLOOKUP(E55,PINS!E$11:F$25,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56">
+        <f>VLOOKUP(C56,PINS!E$11:F$25,2,0)</f>
+        <v>21</v>
+      </c>
+      <c r="E56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56">
+        <f>VLOOKUP(E56,PINS!E$11:F$25,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57">
+        <f>VLOOKUP(C57,PINS!E$11:F$25,2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57">
+        <f>VLOOKUP(E57,PINS!E$11:F$25,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58">
+        <f>VLOOKUP(C58,PINS!E$11:F$25,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58">
+        <f>VLOOKUP(E58,PINS!E$11:F$25,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59">
+        <f>VLOOKUP(C59,PINS!E$11:F$25,2,0)</f>
+        <v>20</v>
+      </c>
+      <c r="E59" t="s">
+        <v>94</v>
+      </c>
+      <c r="F59">
+        <f>VLOOKUP(E59,PINS!E$11:F$25,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60">
+        <f>VLOOKUP(C60,PINS!E$11:F$25,2,0)</f>
+        <v>21</v>
+      </c>
+      <c r="E60" t="s">
+        <v>94</v>
+      </c>
+      <c r="F60">
+        <f>VLOOKUP(E60,PINS!E$11:F$25,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>12</v>
+      </c>
+      <c r="C61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61">
+        <f>VLOOKUP(C61,PINS!E$11:F$25,2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61">
+        <f>VLOOKUP(E61,PINS!E$11:F$25,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62">
+        <f>VLOOKUP(C62,PINS!E$11:F$25,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62">
+        <f>VLOOKUP(E62,PINS!E$11:F$25,2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>4</v>
+      </c>
+      <c r="B63">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63">
+        <f>VLOOKUP(C63,PINS!E$11:F$25,2,0)</f>
+        <v>20</v>
+      </c>
+      <c r="E63" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63">
+        <f>VLOOKUP(E63,PINS!E$11:F$25,2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64">
+        <f>VLOOKUP(C64,PINS!E$11:F$25,2,0)</f>
+        <v>21</v>
+      </c>
+      <c r="E64" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64">
+        <f>VLOOKUP(E64,PINS!E$11:F$25,2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>16</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65">
+        <f>VLOOKUP(C65,PINS!E$11:F$25,2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65">
+        <f>VLOOKUP(E65,PINS!E$11:F$25,2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1313,7 +2404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1336,7 +2427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1348,7 +2439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M63"/>
   <sheetViews>

</xml_diff>